<commit_message>
summerized points from groups and playoff and write it to result.txt
</commit_message>
<xml_diff>
--- a/quizes/solution.xlsx
+++ b/quizes/solution.xlsx
@@ -1,31 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fredriknystrom/python/FIFAWorldCupTip/quizes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredr\python\FIFAWorldCupTip\quizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56A2CAD-1122-DB4E-93C6-1B9F4FA8DDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C96EAD-7EE7-4F43-8884-DCB74DB9A84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34240" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VM Quiz 2022" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -371,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -403,11 +400,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -417,12 +423,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -729,24 +729,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="39" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -786,7 +786,7 @@
       </c>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -794,10 +794,10 @@
         <v>14</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ref="E3:E8" si="0">IF(C3 &gt; D3, 1, IF(D3 &gt; C3, 2, "X"))</f>
@@ -812,19 +812,19 @@
       </c>
       <c r="I3" s="1">
         <f>SUM(C3, C4, C5)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J3" s="1">
         <f>SUM(D3, D4, D5)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K3" s="1">
         <f>SUM(I3, -J3)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L3" s="1">
         <f>SUM(H3*1000, K3, I3*0.001)</f>
-        <v>9003.0030000000006</v>
+        <v>9006.009</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>15</v>
@@ -854,16 +854,16 @@
       <c r="AA3" s="2"/>
       <c r="AC3" s="2" t="str">
         <f>IF(Z4 &gt; AA4, X4, Y4)</f>
-        <v>Argentina</v>
+        <v>Qatar</v>
       </c>
       <c r="AD3" s="2" t="str">
         <f>IF(Z8 &gt; AA8, X8, Y8)</f>
-        <v>Brasilien</v>
+        <v>Spanien</v>
       </c>
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -871,10 +871,10 @@
         <v>19</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
@@ -885,23 +885,23 @@
       </c>
       <c r="H4" s="1">
         <f>SUM(IF(E3 = 2, 3, IF(E3 = "X", 1, 0)), IF(E6 = 1, 3, IF(E6 = "X", 1, 0)), IF(E7 = 1, 3, IF(E7 = "X", 1, 0)))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1">
         <f>SUM(D3, C6, C7)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" s="1">
         <f>SUM(C3, D6, D7)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K4" s="1">
         <f>SUM(I4, -J4)</f>
-        <v>1</v>
+        <v>-3</v>
       </c>
       <c r="L4" s="1">
         <f>SUM(H4*1000, K4, I4*0.001)</f>
-        <v>6001.0020000000004</v>
+        <v>1997.0029999999999</v>
       </c>
       <c r="N4" s="2" t="str">
         <f>INDEX(G3:G6,MATCH(LARGE(L3:L6,1),L3:L6,0))</f>
@@ -909,32 +909,44 @@
       </c>
       <c r="O4" s="2" t="str">
         <f>INDEX(G11:G14,MATCH(LARGE(L11:L14,2),L11:L14,0))</f>
-        <v>England</v>
-      </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+        <v>Wales</v>
+      </c>
+      <c r="P4" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
       <c r="S4" s="2" t="str">
         <f>IF(P4 &gt; Q4, N4, O4)</f>
-        <v>England</v>
+        <v>Qatar</v>
       </c>
       <c r="T4" s="2" t="str">
         <f>IF(P8 &gt; Q8, N8, O8)</f>
-        <v>Ecuador</v>
-      </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
+        <v>England</v>
+      </c>
+      <c r="U4" s="2">
+        <v>2</v>
+      </c>
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
       <c r="X4" s="2" t="str">
         <f>IF(U4 &gt; V4, S4, T4)</f>
-        <v>Ecuador</v>
+        <v>Qatar</v>
       </c>
       <c r="Y4" s="2" t="str">
         <f>IF(U8 &gt; V8, S8, T8)</f>
         <v>Argentina</v>
       </c>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="Z4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -942,10 +954,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
@@ -956,26 +968,26 @@
       </c>
       <c r="H5" s="1">
         <f>SUM(IF(E4 = 2, 3, IF(E4 = "X", 1, 0)), IF(E6 = 2, 3, IF(E6 = "X", 1, 0)), IF(E8 = 1, 3, IF(E8 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="1">
         <f>SUM(D4, D6, C8)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" s="1">
         <f>SUM(C4, C6, D8)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K5" s="1">
         <f>SUM(I5, -J5)</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="L5" s="1">
         <f>SUM(H5*1000, K5, I5*0.001)</f>
-        <v>2999.0010000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+        <v>997.00199999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -986,22 +998,22 @@
         <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="1">
         <f>SUM(IF(E5 = 2, 3, IF(E5 = "X", 1, 0)), IF(E7 = 2, 3, IF(E7 = "X", 1, 0)), IF(E8 = 2, 3, IF(E8 = "X", 1, 0)))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6" s="1">
         <f>SUM(D5, D7, D8)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J6" s="1">
         <f>SUM(C5, C7, C8)</f>
@@ -1009,14 +1021,14 @@
       </c>
       <c r="K6" s="1">
         <f>SUM(I6, -J6)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="L6" s="1">
         <f>SUM(H6*1000, K6, I6*0.001)</f>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+        <v>4000.0030000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1027,11 +1039,11 @@
         <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>21</v>
@@ -1060,7 +1072,7 @@
       </c>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1068,14 +1080,14 @@
         <v>20</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8" s="2" t="str">
         <f>INDEX(G11:G14,MATCH(LARGE(L11:L14,1),L11:L14,0))</f>
@@ -1083,20 +1095,28 @@
       </c>
       <c r="O8" s="2" t="str">
         <f>INDEX(G3:G6,MATCH(LARGE(L3:L6,2),L3:L6,0))</f>
-        <v>Ecuador</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
+        <v>Nederländerna</v>
+      </c>
+      <c r="P8" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1</v>
+      </c>
       <c r="S8" s="2" t="str">
         <f>IF(P12 &gt; Q12, N12, O12)</f>
-        <v>Frankrike</v>
+        <v>Argentina</v>
       </c>
       <c r="T8" s="2" t="str">
         <f>IF(P16 &gt; Q16, N16, O16)</f>
-        <v>Argentina</v>
-      </c>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
+        <v>Frankrike</v>
+      </c>
+      <c r="U8" s="2">
+        <v>2</v>
+      </c>
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
       <c r="X8" s="2" t="str">
         <f>IF(U12 &gt; V12, S12, T12)</f>
         <v>Spanien</v>
@@ -1105,18 +1125,22 @@
         <f>IF(U16 &gt; V16, S16, T16)</f>
         <v>Brasilien</v>
       </c>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="Z8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="12"/>
       <c r="E10" s="3" t="s">
         <v>2</v>
       </c>
@@ -1139,41 +1163,45 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="str">
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
         <f t="shared" ref="E11:E16" si="1">IF(C11 &gt; D11, 1, IF(D11 &gt; C11, 2, "X"))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="3">
         <f>SUM(IF(E11 = 1, 3, IF(E11 = "X", 1, 0)), IF(E12 = 1, 3, IF(E12 = "X", 1, 0)), IF(E13 = 1, 3, IF(E13 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I11" s="3">
         <f>SUM(C11, C12, C13)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J11" s="3">
         <f>SUM(D11, D12, D13)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K11" s="3">
         <f>SUM(I11, -J11)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L11" s="3">
         <f>SUM(H11*1000, K11, I11*0.001)</f>
-        <v>3000</v>
+        <v>9006.009</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>29</v>
@@ -1194,41 +1222,45 @@
       </c>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="str">
+      <c r="C12" s="10">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
         <f t="shared" si="1"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H12" s="3">
         <f>SUM(IF(E11 = 2, 3, IF(E11 = "X", 1, 0)), IF(E14 = 1, 3, IF(E14 = "X", 1, 0)), IF(E15 = 1, 3, IF(E15 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I12" s="3">
         <f>SUM(D11, C14, C15)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J12" s="3">
         <f>SUM(C11, D14, D15)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K12" s="3">
         <f>SUM(I12, -J12)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L12" s="3">
         <f>SUM(H12*1000, K12, I12*0.001)</f>
-        <v>3000</v>
+        <v>1997.0029999999999</v>
       </c>
       <c r="N12" s="2" t="str">
         <f>INDEX(G19:G22,MATCH(LARGE(L19:L22,1),L19:L22,0))</f>
@@ -1236,67 +1268,83 @@
       </c>
       <c r="O12" s="2" t="str">
         <f>INDEX(G27:G30,MATCH(LARGE(L27:L30,2),L27:L30,0))</f>
-        <v>Frankrike</v>
-      </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
+        <v>Tunisien</v>
+      </c>
+      <c r="P12" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>1</v>
+      </c>
       <c r="S12" s="2" t="str">
         <f>IF(P20 &gt; Q20, N20, O20)</f>
-        <v>Belgien</v>
+        <v>Spanien</v>
       </c>
       <c r="T12" s="2" t="str">
         <f>IF(P24 &gt; Q24, N24, O24)</f>
-        <v>Spanien</v>
-      </c>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+        <v>Belgien</v>
+      </c>
+      <c r="U12" s="2">
+        <v>2</v>
+      </c>
+      <c r="V12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="str">
+      <c r="C13" s="10">
+        <v>2</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>32</v>
       </c>
       <c r="H13" s="3">
         <f>SUM(IF(E12 = 2, 3, IF(E12 = "X", 1, 0)), IF(E14 = 2, 3, IF(E14 = "X", 1, 0)), IF(E16 = 1, 3, IF(E16 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I13" s="3">
         <f>SUM(D12, D14, C16)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="3">
         <f>SUM(C12, C14, D16)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K13" s="3">
         <f>SUM(I13, -J13)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L13" s="3">
         <f>SUM(H13*1000, K13, I13*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+        <v>997.00199999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
@@ -1306,15 +1354,15 @@
       </c>
       <c r="H14" s="3">
         <f>SUM(IF(E13 = 2, 3, IF(E13 = "X", 1, 0)), IF(E15 = 2, 3, IF(E15 = "X", 1, 0)), IF(E16 = 2, 3, IF(E16 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14" s="3">
         <f>SUM(D13, D15, D16)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J14" s="3">
         <f>SUM(C13, C15, C16)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K14" s="3">
         <f>SUM(I14, -J14)</f>
@@ -1322,18 +1370,22 @@
       </c>
       <c r="L14" s="3">
         <f>SUM(H14*1000, K14, I14*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+        <v>4000.0030000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1</v>
+      </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
@@ -1357,18 +1409,22 @@
       </c>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="str">
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
         <f t="shared" si="1"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="N16" s="2" t="str">
         <f>INDEX(G27:G30,MATCH(LARGE(L27:L30,1),L27:L30,0))</f>
@@ -1376,30 +1432,38 @@
       </c>
       <c r="O16" s="2" t="str">
         <f>INDEX(G19:G22,MATCH(LARGE(L19:L22,2),L19:L22,0))</f>
-        <v>Argentina</v>
-      </c>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
+        <v>Polen</v>
+      </c>
+      <c r="P16" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1</v>
+      </c>
       <c r="S16" s="2" t="str">
         <f>IF(P28 &gt; Q28, N28, O28)</f>
-        <v>Portugal</v>
+        <v>Brasilien</v>
       </c>
       <c r="T16" s="2" t="str">
         <f>IF(P32 &gt; Q32, N32, O32)</f>
-        <v>Brasilien</v>
-      </c>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="13" t="s">
+        <v>Portugal</v>
+      </c>
+      <c r="U16" s="2">
+        <v>2</v>
+      </c>
+      <c r="V16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="12"/>
       <c r="E18" s="4" t="s">
         <v>2</v>
       </c>
@@ -1422,41 +1486,45 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="str">
+      <c r="C19" s="10">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4">
         <f t="shared" ref="E19:E24" si="2">IF(C19 &gt; D19, 1, IF(D19 &gt; C19, 2, "X"))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>39</v>
       </c>
       <c r="H19" s="4">
         <f>SUM(IF(E19 = 1, 3, IF(E19 = "X", 1, 0)), IF(E20 = 1, 3, IF(E20 = "X", 1, 0)), IF(E21 = 1, 3, IF(E21 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I19" s="4">
         <f>SUM(C19, C20, C21)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J19" s="4">
         <f>SUM(D19, D20, D21)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K19" s="4">
         <f>SUM(I19, -J19)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L19" s="4">
         <f>SUM(H19*1000, K19, I19*0.001)</f>
-        <v>3000</v>
+        <v>9006.009</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>41</v>
@@ -1469,41 +1537,45 @@
       </c>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4" t="str">
+      <c r="C20" s="10">
+        <v>3</v>
+      </c>
+      <c r="D20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
         <f t="shared" si="2"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H20" s="4">
         <f>SUM(IF(E19 = 2, 3, IF(E19 = "X", 1, 0)), IF(E22 = 1, 3, IF(E22 = "X", 1, 0)), IF(E23 = 1, 3, IF(E23 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" s="4">
         <f>SUM(D19, C22, C23)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J20" s="4">
         <f>SUM(C19, D22, D23)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K20" s="4">
         <f>SUM(I20, -J20)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L20" s="4">
         <f>SUM(H20*1000, K20, I20*0.001)</f>
-        <v>3000</v>
+        <v>1997.0029999999999</v>
       </c>
       <c r="N20" s="2" t="str">
         <f>INDEX(G35:G38,MATCH(LARGE(L35:L38,1),L35:L38,0))</f>
@@ -1511,57 +1583,69 @@
       </c>
       <c r="O20" s="2" t="str">
         <f>INDEX(G43:G46,MATCH(LARGE(L43:L46,2),L43:L46,0))</f>
-        <v>Belgien</v>
-      </c>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+        <v>Kroatien</v>
+      </c>
+      <c r="P20" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="str">
+      <c r="C21" s="10">
+        <v>2</v>
+      </c>
+      <c r="D21" s="10">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
         <f t="shared" si="2"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>43</v>
       </c>
       <c r="H21" s="4">
         <f>SUM(IF(E20 = 2, 3, IF(E20 = "X", 1, 0)), IF(E22 = 2, 3, IF(E22 = "X", 1, 0)), IF(E24 = 1, 3, IF(E24 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I21" s="4">
         <f>SUM(D20, D22, C24)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="4">
         <f>SUM(C20, C22, D24)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K21" s="4">
         <f>SUM(I21, -J21)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L21" s="4">
         <f>SUM(H21*1000, K21, I21*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+        <v>997.00199999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="10">
+        <v>1</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1</v>
+      </c>
       <c r="E22" s="4" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
@@ -1571,15 +1655,15 @@
       </c>
       <c r="H22" s="4">
         <f>SUM(IF(E21 = 2, 3, IF(E21 = "X", 1, 0)), IF(E23 = 2, 3, IF(E23 = "X", 1, 0)), IF(E24 = 2, 3, IF(E24 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I22" s="4">
         <f>SUM(D21, D23, D24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J22" s="4">
         <f>SUM(C21, C23, C24)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K22" s="4">
         <f>SUM(I22, -J22)</f>
@@ -1587,18 +1671,22 @@
       </c>
       <c r="L22" s="4">
         <f>SUM(H22*1000, K22, I22*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+        <v>4000.0030000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+      <c r="D23" s="10">
+        <v>1</v>
+      </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
@@ -1614,18 +1702,22 @@
       </c>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4" t="str">
+      <c r="C24" s="10">
+        <v>0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4">
         <f t="shared" si="2"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="N24" s="2" t="str">
         <f>INDEX(G43:G46,MATCH(LARGE(L43:L46,1),L43:L46,0))</f>
@@ -1633,20 +1725,24 @@
       </c>
       <c r="O24" s="2" t="str">
         <f>INDEX(G35:G38,MATCH(LARGE(L35:L38,2),L35:L38,0))</f>
-        <v>Spanien</v>
-      </c>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
+        <v>Japan</v>
+      </c>
+      <c r="P24" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12"/>
       <c r="E26" s="5" t="s">
         <v>2</v>
       </c>
@@ -1669,41 +1765,45 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5" t="str">
+      <c r="C27" s="10">
+        <v>4</v>
+      </c>
+      <c r="D27" s="10">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
         <f t="shared" ref="E27:E32" si="3">IF(C27 &gt; D27, 1, IF(D27 &gt; C27, 2, "X"))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>49</v>
       </c>
       <c r="H27" s="5">
         <f>SUM(IF(E27 = 1, 3, IF(E27 = "X", 1, 0)), IF(E28 = 1, 3, IF(E28 = "X", 1, 0)), IF(E29 = 1, 3, IF(E29 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I27" s="5">
         <f>SUM(C27, C28, C29)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J27" s="5">
         <f>SUM(D27, D28, D29)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K27" s="5">
         <f>SUM(I27, -J27)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L27" s="5">
         <f>SUM(H27*1000, K27, I27*0.001)</f>
-        <v>3000</v>
+        <v>9006.009</v>
       </c>
       <c r="N27" s="2" t="s">
         <v>51</v>
@@ -1716,41 +1816,45 @@
       </c>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="str">
+      <c r="C28" s="10">
+        <v>3</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>50</v>
       </c>
       <c r="H28" s="5">
         <f>SUM(IF(E27 = 2, 3, IF(E27 = "X", 1, 0)), IF(E30 = 1, 3, IF(E30 = "X", 1, 0)), IF(E31 = 1, 3, IF(E31 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I28" s="5">
         <f>SUM(D27, C30, C31)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J28" s="5">
         <f>SUM(C27, D30, D31)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K28" s="5">
         <f>SUM(I28, -J28)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L28" s="5">
         <f>SUM(H28*1000, K28, I28*0.001)</f>
-        <v>3000</v>
+        <v>1997.0029999999999</v>
       </c>
       <c r="N28" s="2" t="str">
         <f>INDEX(G51:G54,MATCH(LARGE(L51:L54,1),L51:L54,0))</f>
@@ -1758,57 +1862,69 @@
       </c>
       <c r="O28" s="2" t="str">
         <f>INDEX(G59:G62,MATCH(LARGE(L59:L62,2),L59:L62,0))</f>
-        <v>Portugal</v>
-      </c>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+        <v>Sydkorea</v>
+      </c>
+      <c r="P28" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="str">
+      <c r="C29" s="10">
+        <v>2</v>
+      </c>
+      <c r="D29" s="10">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>53</v>
       </c>
       <c r="H29" s="5">
         <f>SUM(IF(E28 = 2, 3, IF(E28 = "X", 1, 0)), IF(E30 = 2, 3, IF(E30 = "X", 1, 0)), IF(E32 = 1, 3, IF(E32 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I29" s="5">
         <f>SUM(D28, D30, C32)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J29" s="5">
         <f>SUM(C28, C30, D32)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K29" s="5">
         <f>SUM(I29, -J29)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L29" s="5">
         <f>SUM(H29*1000, K29, I29*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+        <v>997.00199999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="10">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1</v>
+      </c>
       <c r="E30" s="5" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
@@ -1818,15 +1934,15 @@
       </c>
       <c r="H30" s="5">
         <f>SUM(IF(E29 = 2, 3, IF(E29 = "X", 1, 0)), IF(E31 = 2, 3, IF(E31 = "X", 1, 0)), IF(E32 = 2, 3, IF(E32 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I30" s="5">
         <f>SUM(D29, D31, D32)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J30" s="5">
         <f>SUM(C29, C31, C32)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K30" s="5">
         <f>SUM(I30, -J30)</f>
@@ -1834,18 +1950,22 @@
       </c>
       <c r="L30" s="5">
         <f>SUM(H30*1000, K30, I30*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+        <v>4000.0030000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="C31" s="10">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10">
+        <v>1</v>
+      </c>
       <c r="E31" s="5" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
@@ -1861,18 +1981,22 @@
       </c>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5" t="str">
+      <c r="C32" s="10">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1</v>
+      </c>
+      <c r="E32" s="5">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="N32" s="2" t="str">
         <f>INDEX(G59:G62,MATCH(LARGE(L59:L62,1),L59:L62,0))</f>
@@ -1880,20 +2004,24 @@
       </c>
       <c r="O32" s="2" t="str">
         <f>INDEX(G51:G54,MATCH(LARGE(L51:L54,2),L51:L54,0))</f>
-        <v>Brasilien</v>
-      </c>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
+        <v>Kamerun</v>
+      </c>
+      <c r="P32" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="11"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="12"/>
       <c r="E34" s="6" t="s">
         <v>2</v>
       </c>
@@ -1916,126 +2044,142 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6" t="str">
+      <c r="C35" s="10">
+        <v>4</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6">
         <f t="shared" ref="E35:E40" si="4">IF(C35 &gt; D35, 1, IF(D35 &gt; C35, 2, "X"))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>59</v>
       </c>
       <c r="H35" s="6">
         <f>SUM(IF(E35 = 1, 3, IF(E35 = "X", 1, 0)), IF(E36 = 1, 3, IF(E36 = "X", 1, 0)), IF(E37 = 1, 3, IF(E37 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I35" s="6">
         <f>SUM(C35, C36, C37)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J35" s="6">
         <f>SUM(D35, D36, D37)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K35" s="6">
         <f>SUM(I35, -J35)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L35" s="6">
         <f>SUM(H35*1000, K35, I35*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9006.009</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6" t="str">
+      <c r="C36" s="10">
+        <v>3</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1</v>
+      </c>
+      <c r="E36" s="6">
         <f t="shared" si="4"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>60</v>
       </c>
       <c r="H36" s="6">
         <f>SUM(IF(E35 = 2, 3, IF(E35 = "X", 1, 0)), IF(E38 = 1, 3, IF(E38 = "X", 1, 0)), IF(E39 = 1, 3, IF(E39 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I36" s="6">
         <f>SUM(D35, C38, C39)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J36" s="6">
         <f>SUM(C35, D38, D39)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K36" s="6">
         <f>SUM(I36, -J36)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L36" s="6">
         <f>SUM(H36*1000, K36, I36*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1997.0029999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6" t="str">
+      <c r="C37" s="10">
+        <v>2</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1</v>
+      </c>
+      <c r="E37" s="6">
         <f t="shared" si="4"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>61</v>
       </c>
       <c r="H37" s="6">
         <f>SUM(IF(E36 = 2, 3, IF(E36 = "X", 1, 0)), IF(E38 = 2, 3, IF(E38 = "X", 1, 0)), IF(E40 = 1, 3, IF(E40 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I37" s="6">
         <f>SUM(D36, D38, C40)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37" s="6">
         <f>SUM(C36, C38, D40)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K37" s="6">
         <f>SUM(I37, -J37)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L37" s="6">
         <f>SUM(H37*1000, K37, I37*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>997.00199999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="C38" s="10">
+        <v>1</v>
+      </c>
+      <c r="D38" s="10">
+        <v>1</v>
+      </c>
       <c r="E38" s="6" t="str">
         <f t="shared" si="4"/>
         <v>X</v>
@@ -2045,15 +2189,15 @@
       </c>
       <c r="H38" s="6">
         <f>SUM(IF(E37 = 2, 3, IF(E37 = "X", 1, 0)), IF(E39 = 2, 3, IF(E39 = "X", 1, 0)), IF(E40 = 2, 3, IF(E40 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I38" s="6">
         <f>SUM(D37, D39, D40)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J38" s="6">
         <f>SUM(C37, C39, C40)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K38" s="6">
         <f>SUM(I38, -J38)</f>
@@ -2061,46 +2205,54 @@
       </c>
       <c r="L38" s="6">
         <f>SUM(H38*1000, K38, I38*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4000.0030000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="C39" s="10">
+        <v>1</v>
+      </c>
+      <c r="D39" s="10">
+        <v>1</v>
+      </c>
       <c r="E39" s="6" t="str">
         <f t="shared" si="4"/>
         <v>X</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>61</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6" t="str">
+      <c r="C40" s="10">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10">
+        <v>1</v>
+      </c>
+      <c r="E40" s="6">
         <f t="shared" si="4"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="11"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="12"/>
       <c r="E42" s="7" t="s">
         <v>2</v>
       </c>
@@ -2123,126 +2275,142 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7" t="str">
+      <c r="C43" s="10">
+        <v>4</v>
+      </c>
+      <c r="D43" s="10">
+        <v>1</v>
+      </c>
+      <c r="E43" s="7">
         <f t="shared" ref="E43:E48" si="5">IF(C43 &gt; D43, 1, IF(D43 &gt; C43, 2, "X"))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>65</v>
       </c>
       <c r="H43" s="7">
         <f>SUM(IF(E43 = 1, 3, IF(E43 = "X", 1, 0)), IF(E44 = 1, 3, IF(E44 = "X", 1, 0)), IF(E45 = 1, 3, IF(E45 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I43" s="7">
         <f>SUM(C43, C44, C45)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J43" s="7">
         <f>SUM(D43, D44, D45)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K43" s="7">
         <f>SUM(I43, -J43)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L43" s="7">
         <f>SUM(H43*1000, K43, I43*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9006.009</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7" t="str">
+      <c r="C44" s="10">
+        <v>3</v>
+      </c>
+      <c r="D44" s="10">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7">
         <f t="shared" si="5"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>66</v>
       </c>
       <c r="H44" s="7">
         <f>SUM(IF(E43 = 2, 3, IF(E43 = "X", 1, 0)), IF(E46 = 1, 3, IF(E46 = "X", 1, 0)), IF(E47 = 1, 3, IF(E47 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I44" s="7">
         <f>SUM(D43, C46, C47)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J44" s="7">
         <f>SUM(C43, D46, D47)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K44" s="7">
         <f>SUM(I44, -J44)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L44" s="7">
         <f>SUM(H44*1000, K44, I44*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1997.0029999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7" t="str">
+      <c r="C45" s="10">
+        <v>2</v>
+      </c>
+      <c r="D45" s="10">
+        <v>1</v>
+      </c>
+      <c r="E45" s="7">
         <f t="shared" si="5"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>67</v>
       </c>
       <c r="H45" s="7">
         <f>SUM(IF(E44 = 2, 3, IF(E44 = "X", 1, 0)), IF(E46 = 2, 3, IF(E46 = "X", 1, 0)), IF(E48 = 1, 3, IF(E48 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I45" s="7">
         <f>SUM(D44, D46, C48)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J45" s="7">
         <f>SUM(C44, C46, D48)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K45" s="7">
         <f>SUM(I45, -J45)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L45" s="7">
         <f>SUM(H45*1000, K45, I45*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+        <v>997.00199999999995</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
+      <c r="C46" s="10">
+        <v>1</v>
+      </c>
+      <c r="D46" s="10">
+        <v>1</v>
+      </c>
       <c r="E46" s="7" t="str">
         <f t="shared" si="5"/>
         <v>X</v>
@@ -2252,15 +2420,15 @@
       </c>
       <c r="H46" s="7">
         <f>SUM(IF(E45 = 2, 3, IF(E45 = "X", 1, 0)), IF(E47 = 2, 3, IF(E47 = "X", 1, 0)), IF(E48 = 2, 3, IF(E48 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I46" s="7">
         <f>SUM(D45, D47, D48)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J46" s="7">
         <f>SUM(C45, C47, C48)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K46" s="7">
         <f>SUM(I46, -J46)</f>
@@ -2268,46 +2436,54 @@
       </c>
       <c r="L46" s="7">
         <f>SUM(H46*1000, K46, I46*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4000.0030000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7"/>
+      <c r="C47" s="10">
+        <v>1</v>
+      </c>
+      <c r="D47" s="10">
+        <v>1</v>
+      </c>
       <c r="E47" s="7" t="str">
         <f t="shared" si="5"/>
         <v>X</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7" t="str">
+      <c r="C48" s="10">
+        <v>0</v>
+      </c>
+      <c r="D48" s="10">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7">
         <f t="shared" si="5"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="11"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="12"/>
       <c r="E50" s="8" t="s">
         <v>2</v>
       </c>
@@ -2330,126 +2506,142 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8" t="str">
+      <c r="C51" s="10">
+        <v>4</v>
+      </c>
+      <c r="D51" s="10">
+        <v>1</v>
+      </c>
+      <c r="E51" s="8">
         <f t="shared" ref="E51:E56" si="6">IF(C51 &gt; D51, 1, IF(D51 &gt; C51, 2, "X"))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>71</v>
       </c>
       <c r="H51" s="8">
         <f>SUM(IF(E51 = 1, 3, IF(E51 = "X", 1, 0)), IF(E52 = 1, 3, IF(E52 = "X", 1, 0)), IF(E53 = 1, 3, IF(E53 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I51" s="8">
         <f>SUM(C51, C52, C53)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J51" s="8">
         <f>SUM(D51, D52, D53)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K51" s="8">
         <f>SUM(I51, -J51)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L51" s="8">
         <f>SUM(H51*1000, K51, I51*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9006.009</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8" t="str">
+      <c r="C52" s="10">
+        <v>3</v>
+      </c>
+      <c r="D52" s="10">
+        <v>1</v>
+      </c>
+      <c r="E52" s="8">
         <f t="shared" si="6"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>72</v>
       </c>
       <c r="H52" s="8">
         <f>SUM(IF(E51 = 2, 3, IF(E51 = "X", 1, 0)), IF(E54 = 1, 3, IF(E54 = "X", 1, 0)), IF(E55 = 1, 3, IF(E55 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I52" s="8">
         <f>SUM(D51, C54, C55)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J52" s="8">
         <f>SUM(C51, D54, D55)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K52" s="8">
         <f>SUM(I52, -J52)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L52" s="8">
         <f>SUM(H52*1000, K52, I52*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1997.0029999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8" t="str">
+      <c r="C53" s="10">
+        <v>2</v>
+      </c>
+      <c r="D53" s="10">
+        <v>1</v>
+      </c>
+      <c r="E53" s="8">
         <f t="shared" si="6"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G53" s="8" t="s">
         <v>73</v>
       </c>
       <c r="H53" s="8">
         <f>SUM(IF(E52 = 2, 3, IF(E52 = "X", 1, 0)), IF(E54 = 2, 3, IF(E54 = "X", 1, 0)), IF(E56 = 1, 3, IF(E56 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I53" s="8">
         <f>SUM(D52, D54, C56)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J53" s="8">
         <f>SUM(C52, C54, D56)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K53" s="8">
         <f>SUM(I53, -J53)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L53" s="8">
         <f>SUM(H53*1000, K53, I53*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+        <v>997.00199999999995</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
+      <c r="C54" s="10">
+        <v>1</v>
+      </c>
+      <c r="D54" s="10">
+        <v>1</v>
+      </c>
       <c r="E54" s="8" t="str">
         <f t="shared" si="6"/>
         <v>X</v>
@@ -2459,15 +2651,15 @@
       </c>
       <c r="H54" s="8">
         <f>SUM(IF(E53 = 2, 3, IF(E53 = "X", 1, 0)), IF(E55 = 2, 3, IF(E55 = "X", 1, 0)), IF(E56 = 2, 3, IF(E56 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I54" s="8">
         <f>SUM(D53, D55, D56)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J54" s="8">
         <f>SUM(C53, C55, C56)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K54" s="8">
         <f>SUM(I54, -J54)</f>
@@ -2475,46 +2667,54 @@
       </c>
       <c r="L54" s="8">
         <f>SUM(H54*1000, K54, I54*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4000.0030000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
+      <c r="C55" s="10">
+        <v>1</v>
+      </c>
+      <c r="D55" s="10">
+        <v>1</v>
+      </c>
       <c r="E55" s="8" t="str">
         <f t="shared" si="6"/>
         <v>X</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8" t="str">
+      <c r="C56" s="10">
+        <v>0</v>
+      </c>
+      <c r="D56" s="10">
+        <v>1</v>
+      </c>
+      <c r="E56" s="8">
         <f t="shared" si="6"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="11"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="12"/>
       <c r="E58" s="9" t="s">
         <v>2</v>
       </c>
@@ -2537,126 +2737,142 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9" t="str">
+      <c r="C59" s="10">
+        <v>4</v>
+      </c>
+      <c r="D59" s="10">
+        <v>1</v>
+      </c>
+      <c r="E59" s="9">
         <f t="shared" ref="E59:E64" si="7">IF(C59 &gt; D59, 1, IF(D59 &gt; C59, 2, "X"))</f>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>77</v>
       </c>
       <c r="H59" s="9">
         <f>SUM(IF(E59 = 1, 3, IF(E59 = "X", 1, 0)), IF(E60 = 1, 3, IF(E60 = "X", 1, 0)), IF(E61 = 1, 3, IF(E61 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I59" s="9">
         <f>SUM(C59, C60, C61)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J59" s="9">
         <f>SUM(D59, D60, D61)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K59" s="9">
         <f>SUM(I59, -J59)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L59" s="9">
         <f>SUM(H59*1000, K59, I59*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9006.009</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9" t="str">
+      <c r="C60" s="10">
+        <v>3</v>
+      </c>
+      <c r="D60" s="10">
+        <v>1</v>
+      </c>
+      <c r="E60" s="9">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G60" s="9" t="s">
         <v>78</v>
       </c>
       <c r="H60" s="9">
         <f>SUM(IF(E59 = 2, 3, IF(E59 = "X", 1, 0)), IF(E62 = 1, 3, IF(E62 = "X", 1, 0)), IF(E63 = 1, 3, IF(E63 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I60" s="9">
         <f>SUM(D59, C62, C63)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J60" s="9">
         <f>SUM(C59, D62, D63)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K60" s="9">
         <f>SUM(I60, -J60)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L60" s="9">
         <f>SUM(H60*1000, K60, I60*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+        <v>1997.0029999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9" t="str">
+      <c r="C61" s="10">
+        <v>2</v>
+      </c>
+      <c r="D61" s="10">
+        <v>1</v>
+      </c>
+      <c r="E61" s="9">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G61" s="9" t="s">
         <v>79</v>
       </c>
       <c r="H61" s="9">
         <f>SUM(IF(E60 = 2, 3, IF(E60 = "X", 1, 0)), IF(E62 = 2, 3, IF(E62 = "X", 1, 0)), IF(E64 = 1, 3, IF(E64 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I61" s="9">
         <f>SUM(D60, D62, C64)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J61" s="9">
         <f>SUM(C60, C62, D64)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K61" s="9">
         <f>SUM(I61, -J61)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="L61" s="9">
         <f>SUM(H61*1000, K61, I61*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+        <v>997.00199999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C62" s="9"/>
-      <c r="D62" s="9"/>
+      <c r="C62" s="10">
+        <v>1</v>
+      </c>
+      <c r="D62" s="10">
+        <v>1</v>
+      </c>
       <c r="E62" s="9" t="str">
         <f t="shared" si="7"/>
         <v>X</v>
@@ -2666,15 +2882,15 @@
       </c>
       <c r="H62" s="9">
         <f>SUM(IF(E61 = 2, 3, IF(E61 = "X", 1, 0)), IF(E63 = 2, 3, IF(E63 = "X", 1, 0)), IF(E64 = 2, 3, IF(E64 = "X", 1, 0)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I62" s="9">
         <f>SUM(D61, D63, D64)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J62" s="9">
         <f>SUM(C61, C63, C64)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K62" s="9">
         <f>SUM(I62, -J62)</f>
@@ -2682,35 +2898,43 @@
       </c>
       <c r="L62" s="9">
         <f>SUM(H62*1000, K62, I62*0.001)</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4000.0030000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>78</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
+      <c r="C63" s="10">
+        <v>1</v>
+      </c>
+      <c r="D63" s="10">
+        <v>1</v>
+      </c>
       <c r="E63" s="9" t="str">
         <f t="shared" si="7"/>
         <v>X</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>79</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9" t="str">
+      <c r="C64" s="10">
+        <v>0</v>
+      </c>
+      <c r="D64" s="10">
+        <v>1</v>
+      </c>
+      <c r="E64" s="9">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added result to git so that it might be retrievable from javascript
</commit_message>
<xml_diff>
--- a/quizes/solution.xlsx
+++ b/quizes/solution.xlsx
@@ -1,28 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredr\python\FIFAWorldCupTip\quizes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fredriknystrom/python/FIFAWorldCupTip/quizes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C96EAD-7EE7-4F43-8884-DCB74DB9A84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5568C3-6349-D34B-A25C-D4E86BB51E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34240" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VM Quiz 2022" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -400,19 +403,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -423,6 +417,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -729,21 +732,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="39" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="12"/>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="17" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="12"/>
@@ -786,7 +789,7 @@
       </c>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -863,7 +866,7 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -946,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -987,7 +990,7 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>4000.0030000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1075,7 @@
       </c>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1132,12 +1135,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="12"/>
@@ -1163,7 +1166,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1222,7 +1225,7 @@
       </c>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1291,7 +1294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>4000.0030000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1409,7 +1412,7 @@
       </c>
       <c r="V15" s="2"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
@@ -1455,12 +1458,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="12"/>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="19" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="12"/>
@@ -1486,7 +1489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
@@ -1537,7 +1540,7 @@
       </c>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -1592,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>40</v>
       </c>
@@ -1674,7 +1677,7 @@
         <v>4000.0030000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>40</v>
       </c>
@@ -1702,7 +1705,7 @@
       </c>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
@@ -1734,12 +1737,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="12"/>
@@ -1765,7 +1768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>49</v>
       </c>
@@ -1816,7 +1819,7 @@
       </c>
       <c r="Q27" s="2"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>49</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>49</v>
       </c>
@@ -1912,7 +1915,7 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>50</v>
       </c>
@@ -1953,7 +1956,7 @@
         <v>4000.0030000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>50</v>
       </c>
@@ -1981,7 +1984,7 @@
       </c>
       <c r="Q31" s="2"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>53</v>
       </c>
@@ -2013,12 +2016,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="12"/>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="12"/>
@@ -2044,7 +2047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>59</v>
       </c>
@@ -2085,7 +2088,7 @@
         <v>9006.009</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>59</v>
       </c>
@@ -2126,7 +2129,7 @@
         <v>1997.0029999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
         <v>59</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>60</v>
       </c>
@@ -2208,7 +2211,7 @@
         <v>4000.0030000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>60</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
         <v>61</v>
       </c>
@@ -2244,12 +2247,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="16" t="s">
         <v>63</v>
       </c>
       <c r="B42" s="12"/>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D42" s="12"/>
@@ -2275,7 +2278,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>65</v>
       </c>
@@ -2316,7 +2319,7 @@
         <v>9006.009</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>65</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>1997.0029999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>65</v>
       </c>
@@ -2398,7 +2401,7 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>66</v>
       </c>
@@ -2439,7 +2442,7 @@
         <v>4000.0030000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>66</v>
       </c>
@@ -2457,7 +2460,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>67</v>
       </c>
@@ -2475,12 +2478,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B50" s="12"/>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="12"/>
@@ -2506,7 +2509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
         <v>71</v>
       </c>
@@ -2547,7 +2550,7 @@
         <v>9006.009</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
         <v>71</v>
       </c>
@@ -2588,7 +2591,7 @@
         <v>1997.0029999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>71</v>
       </c>
@@ -2629,7 +2632,7 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
         <v>72</v>
       </c>
@@ -2670,7 +2673,7 @@
         <v>4000.0030000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>72</v>
       </c>
@@ -2688,7 +2691,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>73</v>
       </c>
@@ -2706,12 +2709,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A58" s="13" t="s">
         <v>75</v>
       </c>
       <c r="B58" s="12"/>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D58" s="12"/>
@@ -2737,7 +2740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>77</v>
       </c>
@@ -2778,7 +2781,7 @@
         <v>9006.009</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>77</v>
       </c>
@@ -2819,7 +2822,7 @@
         <v>1997.0029999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>77</v>
       </c>
@@ -2860,7 +2863,7 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>78</v>
       </c>
@@ -2901,7 +2904,7 @@
         <v>4000.0030000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>78</v>
       </c>
@@ -2919,7 +2922,7 @@
         <v>X</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>79</v>
       </c>
@@ -2939,6 +2942,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="A50:B50"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="A58:B58"/>
@@ -2949,12 +2958,6 @@
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added top scorer/most goals, changed background colors, removed bugged merged cells
</commit_message>
<xml_diff>
--- a/quizes/solution.xlsx
+++ b/quizes/solution.xlsx
@@ -1,31 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fredriknystrom/python/FIFAWorldCupTip/quizes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredr\python\worldcup\quizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5568C3-6349-D34B-A25C-D4E86BB51E9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5E6D1D-E347-4A5A-9B5E-389171AE5075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34240" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VM Quiz 2022" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="85">
   <si>
     <t>Matches Group A</t>
   </si>
@@ -110,6 +107,15 @@
     <t>Semifinal 2</t>
   </si>
   <si>
+    <t>Winner</t>
+  </si>
+  <si>
+    <t>Top Scorer</t>
+  </si>
+  <si>
+    <t>Goals Scored</t>
+  </si>
+  <si>
     <t>Matches Group B</t>
   </si>
   <si>
@@ -276,6 +282,9 @@
   </si>
   <si>
     <t>Sydkorea</t>
+  </si>
+  <si>
+    <t>Neymar</t>
   </si>
 </sst>
 </file>
@@ -300,7 +309,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF4500"/>
+        <fgColor rgb="FFFB4D3D"/>
       </patternFill>
     </fill>
     <fill>
@@ -310,7 +319,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF8C00"/>
+        <fgColor rgb="FFF7C548"/>
       </patternFill>
     </fill>
     <fill>
@@ -320,27 +329,27 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD700"/>
+        <fgColor rgb="FF226F54"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA9A9A9"/>
+        <fgColor rgb="FFFF8811"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEE82EE"/>
+        <fgColor rgb="FFCB769E"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF87CEEB"/>
+        <fgColor rgb="FF7CDEDC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF888888"/>
+        <fgColor rgb="FF8D99AE"/>
       </patternFill>
     </fill>
   </fills>
@@ -371,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -398,34 +407,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -732,24 +713,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="39" width="15" customWidth="1"/>
+    <col min="1" max="11" width="15" customWidth="1"/>
+    <col min="12" max="12" width="15" hidden="1" customWidth="1"/>
+    <col min="13" max="39" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
@@ -789,7 +772,7 @@
       </c>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -797,7 +780,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -811,23 +794,23 @@
       </c>
       <c r="H3" s="1">
         <f>SUM(IF(E3 = 1, 3, IF(E3 = "X", 1, 0)), IF(E4 = 1, 3, IF(E4 = "X", 1, 0)), IF(E5 = 1, 3, IF(E5 = "X", 1, 0)))</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I3" s="1">
         <f>SUM(C3, C4, C5)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J3" s="1">
         <f>SUM(D3, D4, D5)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K3" s="1">
         <f>SUM(I3, -J3)</f>
-        <v>6</v>
+        <v>-1</v>
       </c>
       <c r="L3" s="1">
         <f>SUM(H3*1000, K3, I3*0.001)</f>
-        <v>9006.009</v>
+        <v>3999.0050000000001</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>15</v>
@@ -857,16 +840,20 @@
       <c r="AA3" s="2"/>
       <c r="AC3" s="2" t="str">
         <f>IF(Z4 &gt; AA4, X4, Y4)</f>
-        <v>Qatar</v>
+        <v>Frankrike</v>
       </c>
       <c r="AD3" s="2" t="str">
         <f>IF(Z8 &gt; AA8, X8, Y8)</f>
-        <v>Spanien</v>
-      </c>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+        <v>Brasilien</v>
+      </c>
+      <c r="AE3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -874,82 +861,82 @@
         <v>19</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="1">
         <f>SUM(IF(E3 = 2, 3, IF(E3 = "X", 1, 0)), IF(E6 = 1, 3, IF(E6 = "X", 1, 0)), IF(E7 = 1, 3, IF(E7 = "X", 1, 0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1">
         <f>SUM(D3, C6, C7)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J4" s="1">
         <f>SUM(C3, D6, D7)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K4" s="1">
         <f>SUM(I4, -J4)</f>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="L4" s="1">
         <f>SUM(H4*1000, K4, I4*0.001)</f>
-        <v>1997.0029999999999</v>
+        <v>2999.0039999999999</v>
       </c>
       <c r="N4" s="2" t="str">
         <f>INDEX(G3:G6,MATCH(LARGE(L3:L6,1),L3:L6,0))</f>
-        <v>Qatar</v>
+        <v>Nederländerna</v>
       </c>
       <c r="O4" s="2" t="str">
         <f>INDEX(G11:G14,MATCH(LARGE(L11:L14,2),L11:L14,0))</f>
         <v>Wales</v>
       </c>
       <c r="P4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="2">
         <v>1</v>
       </c>
       <c r="S4" s="2" t="str">
         <f>IF(P4 &gt; Q4, N4, O4)</f>
-        <v>Qatar</v>
+        <v>Nederländerna</v>
       </c>
       <c r="T4" s="2" t="str">
         <f>IF(P8 &gt; Q8, N8, O8)</f>
         <v>England</v>
       </c>
       <c r="U4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X4" s="2" t="str">
         <f>IF(U4 &gt; V4, S4, T4)</f>
-        <v>Qatar</v>
+        <v>England</v>
       </c>
       <c r="Y4" s="2" t="str">
         <f>IF(U8 &gt; V8, S8, T8)</f>
-        <v>Argentina</v>
+        <v>Frankrike</v>
       </c>
       <c r="Z4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -957,14 +944,14 @@
         <v>20</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>19</v>
@@ -975,11 +962,11 @@
       </c>
       <c r="I5" s="1">
         <f>SUM(D4, D6, C8)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5" s="1">
         <f>SUM(C4, C6, D8)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K5" s="1">
         <f>SUM(I5, -J5)</f>
@@ -987,10 +974,10 @@
       </c>
       <c r="L5" s="1">
         <f>SUM(H5*1000, K5, I5*0.001)</f>
-        <v>997.00199999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+        <v>997.00300000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -998,40 +985,40 @@
         <v>19</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="str">
+      <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="1">
         <f>SUM(IF(E5 = 2, 3, IF(E5 = "X", 1, 0)), IF(E7 = 2, 3, IF(E7 = "X", 1, 0)), IF(E8 = 2, 3, IF(E8 = "X", 1, 0)))</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I6" s="1">
         <f>SUM(D5, D7, D8)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J6" s="1">
         <f>SUM(C5, C7, C8)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" s="1">
         <f>SUM(I6, -J6)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L6" s="1">
         <f>SUM(H6*1000, K6, I6*0.001)</f>
-        <v>4000.0030000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+        <v>9005.0069999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1042,11 +1029,11 @@
         <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="str">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>21</v>
@@ -1074,8 +1061,17 @@
         <v>1</v>
       </c>
       <c r="AA7" s="2"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="AC7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -1086,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
@@ -1098,7 +1094,7 @@
       </c>
       <c r="O8" s="2" t="str">
         <f>INDEX(G3:G6,MATCH(LARGE(L3:L6,2),L3:L6,0))</f>
-        <v>Nederländerna</v>
+        <v>Qatar</v>
       </c>
       <c r="P8" s="2">
         <v>2</v>
@@ -1115,10 +1111,10 @@
         <v>Frankrike</v>
       </c>
       <c r="U8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X8" s="2" t="str">
         <f>IF(U12 &gt; V12, S12, T12)</f>
@@ -1129,26 +1125,36 @@
         <v>Brasilien</v>
       </c>
       <c r="Z8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="12"/>
+        <v>3</v>
+      </c>
+      <c r="AC8" s="2" t="str">
+        <f>IF(AE3 &gt; AF3, AC3, AD3)</f>
+        <v>Brasilien</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>4</v>
@@ -1166,33 +1172,33 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="10">
-        <v>4</v>
-      </c>
-      <c r="D11" s="10">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ref="E11:E16" si="1">IF(C11 &gt; D11, 1, IF(D11 &gt; C11, 2, "X"))</f>
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H11" s="3">
         <f>SUM(IF(E11 = 1, 3, IF(E11 = "X", 1, 0)), IF(E12 = 1, 3, IF(E12 = "X", 1, 0)), IF(E13 = 1, 3, IF(E13 = "X", 1, 0)))</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I11" s="3">
         <f>SUM(C11, C12, C13)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J11" s="3">
         <f>SUM(D11, D12, D13)</f>
@@ -1200,24 +1206,24 @@
       </c>
       <c r="K11" s="3">
         <f>SUM(I11, -J11)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L11" s="3">
         <f>SUM(H11*1000, K11, I11*0.001)</f>
-        <v>9006.009</v>
+        <v>7004.0069999999996</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="S11" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2" t="s">
@@ -1225,17 +1231,17 @@
       </c>
       <c r="V11" s="2"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="10">
-        <v>3</v>
-      </c>
-      <c r="D12" s="10">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
         <v>1</v>
       </c>
       <c r="E12" s="3">
@@ -1243,27 +1249,27 @@
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H12" s="3">
         <f>SUM(IF(E11 = 2, 3, IF(E11 = "X", 1, 0)), IF(E14 = 1, 3, IF(E14 = "X", 1, 0)), IF(E15 = 1, 3, IF(E15 = "X", 1, 0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I12" s="3">
         <f>SUM(D11, C14, C15)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J12" s="3">
         <f>SUM(C11, D14, D15)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K12" s="3">
         <f>SUM(I12, -J12)</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="L12" s="3">
         <f>SUM(H12*1000, K12, I12*0.001)</f>
-        <v>1997.0029999999999</v>
+        <v>2996.0039999999999</v>
       </c>
       <c r="N12" s="2" t="str">
         <f>INDEX(G19:G22,MATCH(LARGE(L19:L22,1),L19:L22,0))</f>
@@ -1271,7 +1277,7 @@
       </c>
       <c r="O12" s="2" t="str">
         <f>INDEX(G27:G30,MATCH(LARGE(L27:L30,2),L27:L30,0))</f>
-        <v>Tunisien</v>
+        <v>Danmark</v>
       </c>
       <c r="P12" s="2">
         <v>2</v>
@@ -1285,34 +1291,34 @@
       </c>
       <c r="T12" s="2" t="str">
         <f>IF(P24 &gt; Q24, N24, O24)</f>
-        <v>Belgien</v>
+        <v>Tyskland</v>
       </c>
       <c r="U12" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V12" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="10">
-        <v>2</v>
-      </c>
-      <c r="D13" s="10">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H13" s="3">
         <f>SUM(IF(E12 = 2, 3, IF(E12 = "X", 1, 0)), IF(E14 = 2, 3, IF(E14 = "X", 1, 0)), IF(E16 = 1, 3, IF(E16 = "X", 1, 0)))</f>
@@ -1320,114 +1326,114 @@
       </c>
       <c r="I13" s="3">
         <f>SUM(D12, D14, C16)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J13" s="3">
         <f>SUM(C12, C14, D16)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K13" s="3">
         <f>SUM(I13, -J13)</f>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="L13" s="3">
         <f>SUM(H13*1000, K13, I13*0.001)</f>
-        <v>997.00199999999995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+        <v>998.00400000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="10">
-        <v>1</v>
-      </c>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="3" t="str">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="3">
+        <f>SUM(IF(E13 = 2, 3, IF(E13 = "X", 1, 0)), IF(E15 = 2, 3, IF(E15 = "X", 1, 0)), IF(E16 = 2, 3, IF(E16 = "X", 1, 0)))</f>
+        <v>5</v>
+      </c>
+      <c r="I14" s="3">
+        <f>SUM(D13, D15, D16)</f>
+        <v>6</v>
+      </c>
+      <c r="J14" s="3">
+        <f>SUM(C13, C15, C16)</f>
+        <v>4</v>
+      </c>
+      <c r="K14" s="3">
+        <f>SUM(I14, -J14)</f>
+        <v>2</v>
+      </c>
+      <c r="L14" s="3">
+        <f>SUM(H14*1000, K14, I14*0.001)</f>
+        <v>5002.0060000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2"/>
+      <c r="S15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>X</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="3">
-        <f>SUM(IF(E13 = 2, 3, IF(E13 = "X", 1, 0)), IF(E15 = 2, 3, IF(E15 = "X", 1, 0)), IF(E16 = 2, 3, IF(E16 = "X", 1, 0)))</f>
-        <v>4</v>
-      </c>
-      <c r="I14" s="3">
-        <f>SUM(D13, D15, D16)</f>
-        <v>3</v>
-      </c>
-      <c r="J14" s="3">
-        <f>SUM(C13, C15, C16)</f>
-        <v>3</v>
-      </c>
-      <c r="K14" s="3">
-        <f>SUM(I14, -J14)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="3">
-        <f>SUM(H14*1000, K14, I14*0.001)</f>
-        <v>4000.0030000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="10">
-        <v>1</v>
-      </c>
-      <c r="D15" s="10">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>X</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="2"/>
-      <c r="S15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" s="2"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="10">
-        <v>0</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="1"/>
-        <v>2</v>
       </c>
       <c r="N16" s="2" t="str">
         <f>INDEX(G27:G30,MATCH(LARGE(L27:L30,1),L27:L30,0))</f>
@@ -1435,10 +1441,10 @@
       </c>
       <c r="O16" s="2" t="str">
         <f>INDEX(G19:G22,MATCH(LARGE(L19:L22,2),L19:L22,0))</f>
-        <v>Polen</v>
+        <v>Mexiko</v>
       </c>
       <c r="P16" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q16" s="2">
         <v>1</v>
@@ -1449,29 +1455,29 @@
       </c>
       <c r="T16" s="2" t="str">
         <f>IF(P32 &gt; Q32, N32, O32)</f>
-        <v>Portugal</v>
+        <v>Uruguay</v>
       </c>
       <c r="U16" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="12"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>4</v>
@@ -1489,25 +1495,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="10">
+        <v>43</v>
+      </c>
+      <c r="C19" s="4">
         <v>4</v>
       </c>
-      <c r="D19" s="10">
-        <v>1</v>
+      <c r="D19" s="4">
+        <v>0</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" ref="E19:E24" si="2">IF(C19 &gt; D19, 1, IF(D19 &gt; C19, 2, "X"))</f>
         <v>1</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H19" s="4">
         <f>SUM(IF(E19 = 1, 3, IF(E19 = "X", 1, 0)), IF(E20 = 1, 3, IF(E20 = "X", 1, 0)), IF(E21 = 1, 3, IF(E21 = "X", 1, 0)))</f>
@@ -1530,27 +1536,27 @@
         <v>9006.009</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="O19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="B20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="10">
-        <v>3</v>
-      </c>
-      <c r="D20" s="10">
+        <v>46</v>
+      </c>
+      <c r="C20" s="4">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
         <v>1</v>
       </c>
       <c r="E20" s="4">
@@ -1558,27 +1564,27 @@
         <v>1</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H20" s="4">
         <f>SUM(IF(E19 = 2, 3, IF(E19 = "X", 1, 0)), IF(E22 = 1, 3, IF(E22 = "X", 1, 0)), IF(E23 = 1, 3, IF(E23 = "X", 1, 0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I20" s="4">
         <f>SUM(D19, C22, C23)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" s="4">
         <f>SUM(C19, D22, D23)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K20" s="4">
         <f>SUM(I20, -J20)</f>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="L20" s="4">
         <f>SUM(H20*1000, K20, I20*0.001)</f>
-        <v>1997.0029999999999</v>
+        <v>-6.9980000000000002</v>
       </c>
       <c r="N20" s="2" t="str">
         <f>INDEX(G35:G38,MATCH(LARGE(L35:L38,1),L35:L38,0))</f>
@@ -1586,171 +1592,171 @@
       </c>
       <c r="O20" s="2" t="str">
         <f>INDEX(G43:G46,MATCH(LARGE(L43:L46,2),L43:L46,0))</f>
-        <v>Kroatien</v>
+        <v>Belgien</v>
       </c>
       <c r="P20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q20" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="10">
-        <v>2</v>
-      </c>
-      <c r="D21" s="10">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4">
+        <v>2</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H21" s="4">
         <f>SUM(IF(E20 = 2, 3, IF(E20 = "X", 1, 0)), IF(E22 = 2, 3, IF(E22 = "X", 1, 0)), IF(E24 = 1, 3, IF(E24 = "X", 1, 0)))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I21" s="4">
         <f>SUM(D20, D22, C24)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J21" s="4">
         <f>SUM(C20, C22, D24)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K21" s="4">
         <f>SUM(I21, -J21)</f>
-        <v>-3</v>
+        <v>3</v>
       </c>
       <c r="L21" s="4">
         <f>SUM(H21*1000, K21, I21*0.001)</f>
-        <v>997.00199999999995</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+        <v>6003.0060000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="10">
-        <v>1</v>
-      </c>
-      <c r="D22" s="10">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4" t="str">
+        <v>46</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3</v>
+      </c>
+      <c r="E22" s="4">
         <f t="shared" si="2"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H22" s="4">
         <f>SUM(IF(E21 = 2, 3, IF(E21 = "X", 1, 0)), IF(E23 = 2, 3, IF(E23 = "X", 1, 0)), IF(E24 = 2, 3, IF(E24 = "X", 1, 0)))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I22" s="4">
         <f>SUM(D21, D23, D24)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J22" s="4">
         <f>SUM(C21, C23, C24)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K22" s="4">
         <f>SUM(I22, -J22)</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="L22" s="4">
         <f>SUM(H22*1000, K22, I22*0.001)</f>
-        <v>4000.0030000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+        <v>2998.0039999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="10">
-        <v>1</v>
-      </c>
-      <c r="D23" s="10">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4" t="str">
+        <v>47</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
         <f t="shared" si="2"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="B24" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="10">
+        <v>47</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
         <v>0</v>
-      </c>
-      <c r="D24" s="10">
-        <v>1</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N24" s="2" t="str">
         <f>INDEX(G43:G46,MATCH(LARGE(L43:L46,1),L43:L46,0))</f>
-        <v>Belgien</v>
+        <v>Kroatien</v>
       </c>
       <c r="O24" s="2" t="str">
         <f>INDEX(G35:G38,MATCH(LARGE(L35:L38,2),L35:L38,0))</f>
-        <v>Japan</v>
+        <v>Tyskland</v>
       </c>
       <c r="P24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D26" s="12"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H26" s="5" t="s">
         <v>4</v>
@@ -1768,17 +1774,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="10">
-        <v>4</v>
-      </c>
-      <c r="D27" s="10">
+        <v>53</v>
+      </c>
+      <c r="C27" s="5">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5">
         <v>1</v>
       </c>
       <c r="E27" s="5">
@@ -1786,7 +1792,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H27" s="5">
         <f>SUM(IF(E27 = 1, 3, IF(E27 = "X", 1, 0)), IF(E28 = 1, 3, IF(E28 = "X", 1, 0)), IF(E29 = 1, 3, IF(E29 = "X", 1, 0)))</f>
@@ -1794,42 +1800,42 @@
       </c>
       <c r="I27" s="5">
         <f>SUM(C27, C28, C29)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J27" s="5">
         <f>SUM(D27, D28, D29)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K27" s="5">
         <f>SUM(I27, -J27)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L27" s="5">
         <f>SUM(H27*1000, K27, I27*0.001)</f>
-        <v>9006.009</v>
+        <v>9005.0069999999996</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="O27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="2"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="P27" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="2"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="B28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="10">
-        <v>3</v>
-      </c>
-      <c r="D28" s="10">
+        <v>56</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2</v>
+      </c>
+      <c r="D28" s="5">
         <v>1</v>
       </c>
       <c r="E28" s="5">
@@ -1837,11 +1843,11 @@
         <v>1</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H28" s="5">
         <f>SUM(IF(E27 = 2, 3, IF(E27 = "X", 1, 0)), IF(E30 = 1, 3, IF(E30 = "X", 1, 0)), IF(E31 = 1, 3, IF(E31 = "X", 1, 0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28" s="5">
         <f>SUM(D27, C30, C31)</f>
@@ -1857,7 +1863,7 @@
       </c>
       <c r="L28" s="5">
         <f>SUM(H28*1000, K28, I28*0.001)</f>
-        <v>1997.0029999999999</v>
+        <v>997.00300000000004</v>
       </c>
       <c r="N28" s="2" t="str">
         <f>INDEX(G51:G54,MATCH(LARGE(L51:L54,1),L51:L54,0))</f>
@@ -1865,108 +1871,108 @@
       </c>
       <c r="O28" s="2" t="str">
         <f>INDEX(G59:G62,MATCH(LARGE(L59:L62,2),L59:L62,0))</f>
-        <v>Sydkorea</v>
+        <v>Portugal</v>
       </c>
       <c r="P28" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q28" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="10">
-        <v>2</v>
-      </c>
-      <c r="D29" s="10">
-        <v>1</v>
+        <v>57</v>
+      </c>
+      <c r="C29" s="5">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
       </c>
       <c r="E29" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H29" s="5">
         <f>SUM(IF(E28 = 2, 3, IF(E28 = "X", 1, 0)), IF(E30 = 2, 3, IF(E30 = "X", 1, 0)), IF(E32 = 1, 3, IF(E32 = "X", 1, 0)))</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I29" s="5">
         <f>SUM(D28, D30, C32)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J29" s="5">
         <f>SUM(C28, C30, D32)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K29" s="5">
         <f>SUM(I29, -J29)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L29" s="5">
         <f>SUM(H29*1000, K29, I29*0.001)</f>
-        <v>997.00199999999995</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+        <v>6002.0050000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="10">
-        <v>1</v>
-      </c>
-      <c r="D30" s="10">
-        <v>1</v>
-      </c>
-      <c r="E30" s="5" t="str">
+        <v>56</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1</v>
+      </c>
+      <c r="D30" s="5">
+        <v>2</v>
+      </c>
+      <c r="E30" s="5">
         <f t="shared" si="3"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H30" s="5">
         <f>SUM(IF(E29 = 2, 3, IF(E29 = "X", 1, 0)), IF(E31 = 2, 3, IF(E31 = "X", 1, 0)), IF(E32 = 2, 3, IF(E32 = "X", 1, 0)))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I30" s="5">
         <f>SUM(D29, D31, D32)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J30" s="5">
         <f>SUM(C29, C31, C32)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K30" s="5">
         <f>SUM(I30, -J30)</f>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="L30" s="5">
         <f>SUM(H30*1000, K30, I30*0.001)</f>
-        <v>4000.0030000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+        <v>996.00099999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="10">
-        <v>1</v>
-      </c>
-      <c r="D31" s="10">
+        <v>57</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1</v>
+      </c>
+      <c r="D31" s="5">
         <v>1</v>
       </c>
       <c r="E31" s="5" t="str">
@@ -1974,62 +1980,62 @@
         <v>X</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="O31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="2"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="P31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="2"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="B32" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="10">
+        <v>57</v>
+      </c>
+      <c r="C32" s="5">
+        <v>2</v>
+      </c>
+      <c r="D32" s="5">
         <v>0</v>
-      </c>
-      <c r="D32" s="10">
-        <v>1</v>
       </c>
       <c r="E32" s="5">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N32" s="2" t="str">
         <f>INDEX(G59:G62,MATCH(LARGE(L59:L62,1),L59:L62,0))</f>
-        <v>Portugal</v>
+        <v>Uruguay</v>
       </c>
       <c r="O32" s="2" t="str">
         <f>INDEX(G51:G54,MATCH(LARGE(L51:L54,2),L51:L54,0))</f>
-        <v>Kamerun</v>
+        <v>Schweiz</v>
       </c>
       <c r="P32" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q32" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" s="12"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="6"/>
       <c r="E34" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>4</v>
@@ -2047,25 +2053,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="10">
+        <v>63</v>
+      </c>
+      <c r="C35" s="6">
         <v>4</v>
       </c>
-      <c r="D35" s="10">
-        <v>1</v>
+      <c r="D35" s="6">
+        <v>0</v>
       </c>
       <c r="E35" s="6">
         <f t="shared" ref="E35:E40" si="4">IF(C35 &gt; D35, 1, IF(D35 &gt; C35, 2, "X"))</f>
         <v>1</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H35" s="6">
         <f>SUM(IF(E35 = 1, 3, IF(E35 = "X", 1, 0)), IF(E36 = 1, 3, IF(E36 = "X", 1, 0)), IF(E37 = 1, 3, IF(E37 = "X", 1, 0)))</f>
@@ -2073,11 +2079,11 @@
       </c>
       <c r="I35" s="6">
         <f>SUM(C35, C36, C37)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J35" s="6">
         <f>SUM(D35, D36, D37)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K35" s="6">
         <f>SUM(I35, -J35)</f>
@@ -2085,61 +2091,61 @@
       </c>
       <c r="L35" s="6">
         <f>SUM(H35*1000, K35, I35*0.001)</f>
-        <v>9006.009</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9006.0069999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="10">
-        <v>3</v>
-      </c>
-      <c r="D36" s="10">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="C36" s="6">
+        <v>1</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0</v>
       </c>
       <c r="E36" s="6">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H36" s="6">
         <f>SUM(IF(E35 = 2, 3, IF(E35 = "X", 1, 0)), IF(E38 = 1, 3, IF(E38 = "X", 1, 0)), IF(E39 = 1, 3, IF(E39 = "X", 1, 0)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I36" s="6">
         <f>SUM(D35, C38, C39)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J36" s="6">
         <f>SUM(C35, D38, D39)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K36" s="6">
         <f>SUM(I36, -J36)</f>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="L36" s="6">
         <f>SUM(H36*1000, K36, I36*0.001)</f>
-        <v>1997.0029999999999</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+        <v>-6.9980000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="10">
-        <v>2</v>
-      </c>
-      <c r="D37" s="10">
+        <v>65</v>
+      </c>
+      <c r="C37" s="6">
+        <v>2</v>
+      </c>
+      <c r="D37" s="6">
         <v>1</v>
       </c>
       <c r="E37" s="6">
@@ -2147,48 +2153,48 @@
         <v>1</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H37" s="6">
         <f>SUM(IF(E36 = 2, 3, IF(E36 = "X", 1, 0)), IF(E38 = 2, 3, IF(E38 = "X", 1, 0)), IF(E40 = 1, 3, IF(E40 = "X", 1, 0)))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I37" s="6">
         <f>SUM(D36, D38, C40)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J37" s="6">
         <f>SUM(C36, C38, D40)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K37" s="6">
         <f>SUM(I37, -J37)</f>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="L37" s="6">
         <f>SUM(H37*1000, K37, I37*0.001)</f>
-        <v>997.00199999999995</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4001.0050000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" s="10">
-        <v>1</v>
-      </c>
-      <c r="D38" s="10">
-        <v>1</v>
-      </c>
-      <c r="E38" s="6" t="str">
+        <v>64</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1</v>
+      </c>
+      <c r="D38" s="6">
+        <v>3</v>
+      </c>
+      <c r="E38" s="6">
         <f t="shared" si="4"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H38" s="6">
         <f>SUM(IF(E37 = 2, 3, IF(E37 = "X", 1, 0)), IF(E39 = 2, 3, IF(E39 = "X", 1, 0)), IF(E40 = 2, 3, IF(E40 = "X", 1, 0)))</f>
@@ -2196,11 +2202,11 @@
       </c>
       <c r="I38" s="6">
         <f>SUM(D37, D39, D40)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J38" s="6">
         <f>SUM(C37, C39, C40)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K38" s="6">
         <f>SUM(I38, -J38)</f>
@@ -2208,59 +2214,59 @@
       </c>
       <c r="L38" s="6">
         <f>SUM(H38*1000, K38, I38*0.001)</f>
-        <v>4000.0030000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4000.0050000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="10">
-        <v>1</v>
-      </c>
-      <c r="D39" s="10">
-        <v>1</v>
-      </c>
-      <c r="E39" s="6" t="str">
+        <v>65</v>
+      </c>
+      <c r="C39" s="6">
+        <v>1</v>
+      </c>
+      <c r="D39" s="6">
+        <v>2</v>
+      </c>
+      <c r="E39" s="6">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="6">
+        <v>2</v>
+      </c>
+      <c r="D40" s="6">
+        <v>2</v>
+      </c>
+      <c r="E40" s="6" t="str">
         <f t="shared" si="4"/>
         <v>X</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="10">
-        <v>0</v>
-      </c>
-      <c r="D40" s="10">
-        <v>1</v>
-      </c>
-      <c r="E40" s="6">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="12"/>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
         <v>2</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H42" s="7" t="s">
         <v>4</v>
@@ -2278,17 +2284,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="10">
-        <v>4</v>
-      </c>
-      <c r="D43" s="10">
+        <v>69</v>
+      </c>
+      <c r="C43" s="7">
+        <v>2</v>
+      </c>
+      <c r="D43" s="7">
         <v>1</v>
       </c>
       <c r="E43" s="7">
@@ -2296,40 +2302,40 @@
         <v>1</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H43" s="7">
         <f>SUM(IF(E43 = 1, 3, IF(E43 = "X", 1, 0)), IF(E44 = 1, 3, IF(E44 = "X", 1, 0)), IF(E45 = 1, 3, IF(E45 = "X", 1, 0)))</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I43" s="7">
         <f>SUM(C43, C44, C45)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J43" s="7">
         <f>SUM(D43, D44, D45)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K43" s="7">
         <f>SUM(I43, -J43)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L43" s="7">
         <f>SUM(H43*1000, K43, I43*0.001)</f>
-        <v>9006.009</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+        <v>7002.0060000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="10">
-        <v>3</v>
-      </c>
-      <c r="D44" s="10">
+        <v>70</v>
+      </c>
+      <c r="C44" s="7">
+        <v>2</v>
+      </c>
+      <c r="D44" s="7">
         <v>1</v>
       </c>
       <c r="E44" s="7">
@@ -2337,11 +2343,11 @@
         <v>1</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H44" s="7">
         <f>SUM(IF(E43 = 2, 3, IF(E43 = "X", 1, 0)), IF(E46 = 1, 3, IF(E46 = "X", 1, 0)), IF(E47 = 1, 3, IF(E47 = "X", 1, 0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I44" s="7">
         <f>SUM(D43, C46, C47)</f>
@@ -2357,28 +2363,28 @@
       </c>
       <c r="L44" s="7">
         <f>SUM(H44*1000, K44, I44*0.001)</f>
-        <v>1997.0029999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+        <v>997.00300000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C45" s="10">
-        <v>2</v>
-      </c>
-      <c r="D45" s="10">
-        <v>1</v>
-      </c>
-      <c r="E45" s="7">
+        <v>71</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2</v>
+      </c>
+      <c r="D45" s="7">
+        <v>2</v>
+      </c>
+      <c r="E45" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H45" s="7">
         <f>SUM(IF(E44 = 2, 3, IF(E44 = "X", 1, 0)), IF(E46 = 2, 3, IF(E46 = "X", 1, 0)), IF(E48 = 1, 3, IF(E48 = "X", 1, 0)))</f>
@@ -2401,17 +2407,17 @@
         <v>997.00199999999995</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="10">
-        <v>1</v>
-      </c>
-      <c r="D46" s="10">
+        <v>70</v>
+      </c>
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="D46" s="7">
         <v>1</v>
       </c>
       <c r="E46" s="7" t="str">
@@ -2419,15 +2425,15 @@
         <v>X</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H46" s="7">
         <f>SUM(IF(E45 = 2, 3, IF(E45 = "X", 1, 0)), IF(E47 = 2, 3, IF(E47 = "X", 1, 0)), IF(E48 = 2, 3, IF(E48 = "X", 1, 0)))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I46" s="7">
         <f>SUM(D45, D47, D48)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J46" s="7">
         <f>SUM(C45, C47, C48)</f>
@@ -2435,63 +2441,63 @@
       </c>
       <c r="K46" s="7">
         <f>SUM(I46, -J46)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L46" s="7">
         <f>SUM(H46*1000, K46, I46*0.001)</f>
-        <v>4000.0030000000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+        <v>7004.0069999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="10">
-        <v>1</v>
-      </c>
-      <c r="D47" s="10">
-        <v>1</v>
-      </c>
-      <c r="E47" s="7" t="str">
+        <v>71</v>
+      </c>
+      <c r="C47" s="7">
+        <v>1</v>
+      </c>
+      <c r="D47" s="7">
+        <v>3</v>
+      </c>
+      <c r="E47" s="7">
         <f t="shared" si="5"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C48" s="10">
+        <v>71</v>
+      </c>
+      <c r="C48" s="7">
         <v>0</v>
       </c>
-      <c r="D48" s="10">
-        <v>1</v>
+      <c r="D48" s="7">
+        <v>2</v>
       </c>
       <c r="E48" s="7">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B50" s="12"/>
-      <c r="C50" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D50" s="12"/>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="8"/>
       <c r="E50" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>4</v>
@@ -2509,17 +2515,17 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="10">
-        <v>4</v>
-      </c>
-      <c r="D51" s="10">
+        <v>75</v>
+      </c>
+      <c r="C51" s="8">
+        <v>3</v>
+      </c>
+      <c r="D51" s="8">
         <v>1</v>
       </c>
       <c r="E51" s="8">
@@ -2527,7 +2533,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H51" s="8">
         <f>SUM(IF(E51 = 1, 3, IF(E51 = "X", 1, 0)), IF(E52 = 1, 3, IF(E52 = "X", 1, 0)), IF(E53 = 1, 3, IF(E53 = "X", 1, 0)))</f>
@@ -2535,32 +2541,32 @@
       </c>
       <c r="I51" s="8">
         <f>SUM(C51, C52, C53)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J51" s="8">
         <f>SUM(D51, D52, D53)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K51" s="8">
         <f>SUM(I51, -J51)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L51" s="8">
         <f>SUM(H51*1000, K51, I51*0.001)</f>
-        <v>9006.009</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+        <v>9008.01</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C52" s="10">
-        <v>3</v>
-      </c>
-      <c r="D52" s="10">
+        <v>76</v>
+      </c>
+      <c r="C52" s="8">
+        <v>2</v>
+      </c>
+      <c r="D52" s="8">
         <v>1</v>
       </c>
       <c r="E52" s="8">
@@ -2568,15 +2574,15 @@
         <v>1</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H52" s="8">
         <f>SUM(IF(E51 = 2, 3, IF(E51 = "X", 1, 0)), IF(E54 = 1, 3, IF(E54 = "X", 1, 0)), IF(E55 = 1, 3, IF(E55 = "X", 1, 0)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I52" s="8">
         <f>SUM(D51, C54, C55)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J52" s="8">
         <f>SUM(C51, D54, D55)</f>
@@ -2584,145 +2590,145 @@
       </c>
       <c r="K52" s="8">
         <f>SUM(I52, -J52)</f>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="L52" s="8">
         <f>SUM(H52*1000, K52, I52*0.001)</f>
-        <v>1997.0029999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2998.0039999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="10">
-        <v>2</v>
-      </c>
-      <c r="D53" s="10">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="C53" s="8">
+        <v>5</v>
+      </c>
+      <c r="D53" s="8">
+        <v>0</v>
       </c>
       <c r="E53" s="8">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H53" s="8">
         <f>SUM(IF(E52 = 2, 3, IF(E52 = "X", 1, 0)), IF(E54 = 2, 3, IF(E54 = "X", 1, 0)), IF(E56 = 1, 3, IF(E56 = "X", 1, 0)))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I53" s="8">
         <f>SUM(D52, D54, C56)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J53" s="8">
         <f>SUM(C52, C54, D56)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K53" s="8">
         <f>SUM(I53, -J53)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="L53" s="8">
         <f>SUM(H53*1000, K53, I53*0.001)</f>
-        <v>997.00199999999995</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4000.0039999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C54" s="10">
-        <v>1</v>
-      </c>
-      <c r="D54" s="10">
-        <v>1</v>
-      </c>
-      <c r="E54" s="8" t="str">
+        <v>76</v>
+      </c>
+      <c r="C54" s="8">
+        <v>1</v>
+      </c>
+      <c r="D54" s="8">
+        <v>2</v>
+      </c>
+      <c r="E54" s="8">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="G54" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H54" s="8">
+        <f>SUM(IF(E53 = 2, 3, IF(E53 = "X", 1, 0)), IF(E55 = 2, 3, IF(E55 = "X", 1, 0)), IF(E56 = 2, 3, IF(E56 = "X", 1, 0)))</f>
+        <v>1</v>
+      </c>
+      <c r="I54" s="8">
+        <f>SUM(D53, D55, D56)</f>
+        <v>2</v>
+      </c>
+      <c r="J54" s="8">
+        <f>SUM(C53, C55, C56)</f>
+        <v>8</v>
+      </c>
+      <c r="K54" s="8">
+        <f>SUM(I54, -J54)</f>
+        <v>-6</v>
+      </c>
+      <c r="L54" s="8">
+        <f>SUM(H54*1000, K54, I54*0.001)</f>
+        <v>994.00199999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" s="8">
+        <v>2</v>
+      </c>
+      <c r="D55" s="8">
+        <v>1</v>
+      </c>
+      <c r="E55" s="8">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="8">
+        <v>1</v>
+      </c>
+      <c r="D56" s="8">
+        <v>1</v>
+      </c>
+      <c r="E56" s="8" t="str">
         <f t="shared" si="6"/>
         <v>X</v>
       </c>
-      <c r="G54" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="H54" s="8">
-        <f>SUM(IF(E53 = 2, 3, IF(E53 = "X", 1, 0)), IF(E55 = 2, 3, IF(E55 = "X", 1, 0)), IF(E56 = 2, 3, IF(E56 = "X", 1, 0)))</f>
-        <v>4</v>
-      </c>
-      <c r="I54" s="8">
-        <f>SUM(D53, D55, D56)</f>
-        <v>3</v>
-      </c>
-      <c r="J54" s="8">
-        <f>SUM(C53, C55, C56)</f>
-        <v>3</v>
-      </c>
-      <c r="K54" s="8">
-        <f>SUM(I54, -J54)</f>
-        <v>0</v>
-      </c>
-      <c r="L54" s="8">
-        <f>SUM(H54*1000, K54, I54*0.001)</f>
-        <v>4000.0030000000002</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C55" s="10">
-        <v>1</v>
-      </c>
-      <c r="D55" s="10">
-        <v>1</v>
-      </c>
-      <c r="E55" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v>X</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C56" s="10">
-        <v>0</v>
-      </c>
-      <c r="D56" s="10">
-        <v>1</v>
-      </c>
-      <c r="E56" s="8">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="12"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="9"/>
       <c r="E58" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H58" s="9" t="s">
         <v>4</v>
@@ -2740,70 +2746,70 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C59" s="10">
-        <v>4</v>
-      </c>
-      <c r="D59" s="10">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="C59" s="9">
+        <v>3</v>
+      </c>
+      <c r="D59" s="9">
+        <v>2</v>
       </c>
       <c r="E59" s="9">
         <f t="shared" ref="E59:E64" si="7">IF(C59 &gt; D59, 1, IF(D59 &gt; C59, 2, "X"))</f>
         <v>1</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="H59" s="9">
         <f>SUM(IF(E59 = 1, 3, IF(E59 = "X", 1, 0)), IF(E60 = 1, 3, IF(E60 = "X", 1, 0)), IF(E61 = 1, 3, IF(E61 = "X", 1, 0)))</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I59" s="9">
         <f>SUM(C59, C60, C61)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J59" s="9">
         <f>SUM(D59, D60, D61)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K59" s="9">
         <f>SUM(I59, -J59)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L59" s="9">
         <f>SUM(H59*1000, K59, I59*0.001)</f>
-        <v>9006.009</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+        <v>7003.0069999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C60" s="10">
-        <v>3</v>
-      </c>
-      <c r="D60" s="10">
-        <v>1</v>
-      </c>
-      <c r="E60" s="9">
+        <v>82</v>
+      </c>
+      <c r="C60" s="9">
+        <v>2</v>
+      </c>
+      <c r="D60" s="9">
+        <v>2</v>
+      </c>
+      <c r="E60" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>X</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H60" s="9">
         <f>SUM(IF(E59 = 2, 3, IF(E59 = "X", 1, 0)), IF(E62 = 1, 3, IF(E62 = "X", 1, 0)), IF(E63 = 1, 3, IF(E63 = "X", 1, 0)))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I60" s="9">
         <f>SUM(D59, C62, C63)</f>
@@ -2811,110 +2817,110 @@
       </c>
       <c r="J60" s="9">
         <f>SUM(C59, D62, D63)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K60" s="9">
         <f>SUM(I60, -J60)</f>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="L60" s="9">
         <f>SUM(H60*1000, K60, I60*0.001)</f>
-        <v>1997.0029999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+        <v>998.00300000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C61" s="10">
-        <v>2</v>
-      </c>
-      <c r="D61" s="10">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="C61" s="9">
+        <v>2</v>
+      </c>
+      <c r="D61" s="9">
+        <v>0</v>
       </c>
       <c r="E61" s="9">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H61" s="9">
         <f>SUM(IF(E60 = 2, 3, IF(E60 = "X", 1, 0)), IF(E62 = 2, 3, IF(E62 = "X", 1, 0)), IF(E64 = 1, 3, IF(E64 = "X", 1, 0)))</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I61" s="9">
         <f>SUM(D60, D62, C64)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J61" s="9">
         <f>SUM(C60, C62, D64)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K61" s="9">
         <f>SUM(I61, -J61)</f>
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="L61" s="9">
         <f>SUM(H61*1000, K61, I61*0.001)</f>
-        <v>997.00199999999995</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+        <v>7004.0060000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C62" s="10">
-        <v>1</v>
-      </c>
-      <c r="D62" s="10">
-        <v>1</v>
-      </c>
-      <c r="E62" s="9" t="str">
+        <v>82</v>
+      </c>
+      <c r="C62" s="9">
+        <v>0</v>
+      </c>
+      <c r="D62" s="9">
+        <v>1</v>
+      </c>
+      <c r="E62" s="9">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v>2</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H62" s="9">
         <f>SUM(IF(E61 = 2, 3, IF(E61 = "X", 1, 0)), IF(E63 = 2, 3, IF(E63 = "X", 1, 0)), IF(E64 = 2, 3, IF(E64 = "X", 1, 0)))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I62" s="9">
         <f>SUM(D61, D63, D64)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J62" s="9">
         <f>SUM(C61, C63, C64)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K62" s="9">
         <f>SUM(I62, -J62)</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="L62" s="9">
         <f>SUM(H62*1000, K62, I62*0.001)</f>
-        <v>4000.0030000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+        <v>995.00099999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63" s="10">
-        <v>1</v>
-      </c>
-      <c r="D63" s="10">
+        <v>83</v>
+      </c>
+      <c r="C63" s="9">
+        <v>1</v>
+      </c>
+      <c r="D63" s="9">
         <v>1</v>
       </c>
       <c r="E63" s="9" t="str">
@@ -2922,43 +2928,25 @@
         <v>X</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C64" s="10">
+        <v>83</v>
+      </c>
+      <c r="C64" s="9">
+        <v>3</v>
+      </c>
+      <c r="D64" s="9">
         <v>0</v>
-      </c>
-      <c r="D64" s="10">
-        <v>1</v>
       </c>
       <c r="E64" s="9">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved final one step down to simplify making of solution algo
</commit_message>
<xml_diff>
--- a/quizes/solution.xlsx
+++ b/quizes/solution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredr\python\worldcup\quizes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5E6D1D-E347-4A5A-9B5E-389171AE5075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7B2079-6AB4-462A-B558-10324E51D4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,7 +714,7 @@
   <dimension ref="A2:AF64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AD20" sqref="AD20"/>
+      <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>